<commit_message>
added x90 to Camera Analysis
</commit_message>
<xml_diff>
--- a/Camera Analysis.xlsx
+++ b/Camera Analysis.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -70,16 +70,16 @@
     <t>Kaiser Baas X2</t>
   </si>
   <si>
-    <t>2016?</t>
-  </si>
-  <si>
-    <t>??</t>
+    <t>MPEG</t>
   </si>
   <si>
     <t>1080p, 720p</t>
   </si>
   <si>
     <t>60, 30 (120 at 720p)</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
   <si>
     <t>https://www.jbhifi.com.au/cameras/video-cameras/kaiser-baas/kaiser-baas-x2-action-camera/388662/</t>
@@ -144,6 +144,15 @@
   <si>
     <t>https://www.olfi.co.uk/</t>
   </si>
+  <si>
+    <t>Kaiser Baas X90</t>
+  </si>
+  <si>
+    <t>90 mins</t>
+  </si>
+  <si>
+    <t>https://www.jbhifi.com.au/cameras/video-cameras/kaiser-baas/kaiser-baas-x90-action-camera/984438/</t>
+  </si>
 </sst>
 </file>
 
@@ -153,7 +162,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -174,6 +183,13 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FFFF0000"/>
     </font>
   </fonts>
   <fills count="3">
@@ -209,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -246,7 +262,19 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -378,23 +406,23 @@
       <c r="A3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="4">
+        <v>2016.0</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E3" s="4">
         <v>170.0</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>16</v>
@@ -432,7 +460,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="8">
         <v>140.0</v>
@@ -444,7 +472,7 @@
         <v>27</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="10">
@@ -472,29 +500,29 @@
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>150.0</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="12">
+      <c r="I5" s="5"/>
+      <c r="J5" s="6">
         <v>99.0</v>
       </c>
       <c r="K5" s="11" t="s">
@@ -519,31 +547,31 @@
       <c r="A6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="6">
         <v>125.0</v>
       </c>
       <c r="K6" s="11" t="s">
@@ -565,17 +593,37 @@
       <c r="Y6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="A7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="13">
+        <v>2016.0</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="13">
+        <v>170.0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>30.0</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15">
+        <v>79.0</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>46</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -27409,7 +27457,8 @@
     <hyperlink r:id="rId3" ref="K4"/>
     <hyperlink r:id="rId4" ref="K5"/>
     <hyperlink r:id="rId5" ref="K6"/>
+    <hyperlink r:id="rId6" ref="K7"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>